<commit_message>
Product List and Email Submitting
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -405,7 +405,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="ProductsData"/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,46 +423,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>GPI-0181</v>
+        <v>GPT-0516</v>
       </c>
       <c r="B2" t="str">
-        <v>EPSON INK T0424 YELLOW ΣΥΜΒΑΤΟ 16ml</v>
+        <v>KONICA MINOLTA TONER 2300 BLACK ΣΥΜΒΑΤΟ 4000 ΣΕΛΙΔΕΣ</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>GPI-0017</v>
+        <v>GPI-0079</v>
       </c>
       <c r="B3" t="str">
-        <v>EPSON INK T01813 MAGENTA ΣΥΜΒΑΤΟ 10ml</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>GPT-0219</v>
-      </c>
-      <c r="B4" t="str">
-        <v>HP TONER MFP CB382A YELLOW ΣΥΜΒΑΤΟ 21000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="C4">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>GPT-0380</v>
-      </c>
-      <c r="B5" t="str">
-        <v>RICOH TONER MFP C811 CYAN ΣΥΜΒΑΤΟ 15000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="C5">
-        <v>76</v>
+        <v>HP INK No 351XL - CB338EE COLOR ΣΥΜΒΑΤΟ 18ml</v>
+      </c>
+      <c r="C3" t="str">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Product Can Be Used Now - Uncompleted
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,40 +421,37 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>APOSTOLIS ANASTASIOU</v>
+        <v>ΤΑΤΣΗΣ  ΓΕΩΡΓΙΟΣ</v>
       </c>
       <c r="B2" t="str">
-        <v>ACS COURIER</v>
+        <v>ΕΛΤΑ COURIER</v>
       </c>
       <c r="C2" t="str">
-        <v>123123123123</v>
+        <v>134312928</v>
       </c>
       <c r="D2" t="str">
-        <v>6975362321</v>
-      </c>
-      <c r="E2" t="str">
-        <v>6975362321</v>
+        <v>2681071591</v>
       </c>
       <c r="F2" t="str">
-        <v>49100</v>
+        <v>47100</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>ΑΡΤΑ</v>
       </c>
       <c r="H2" t="str">
-        <v>Kaiser Bridge</v>
+        <v>ΦΛΕΜΙΝΓΚ ΚΑΙ ΠΕΡΙΦ ΟΔΟΣ 0</v>
       </c>
       <c r="I2" t="str">
-        <v>GPT-0516</v>
+        <v>GPT-0532</v>
       </c>
       <c r="J2" t="str">
-        <v>KONICA MINOLTA TONER 2300 BLACK ΣΥΜΒΑΤΟ 4000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
+        <v>OKI TONER M C3100/3000/3200/5100/5150/5200/5300/5400/5510 MAGENTA ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
+      </c>
+      <c r="K2" t="str">
+        <v>108</v>
       </c>
       <c r="L2" t="str">
-        <v>0€</v>
+        <v>1023.78€</v>
       </c>
     </row>
     <row r="3">
@@ -483,13 +480,13 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>GPT-0516</v>
+        <v>GPI-0134</v>
       </c>
       <c r="J3" t="str">
-        <v>KONICA MINOLTA TONER 2300 BLACK ΣΥΜΒΑΤΟ 4000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
+        <v>HP INK No 88XL -  C9392A MAGENTA ΣΥΜΒΑΤΟ 28ml</v>
+      </c>
+      <c r="K3" t="str">
+        <v>76</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -521,15 +518,53 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>GPT-0516</v>
+        <v>GPI-0023</v>
       </c>
       <c r="J4" t="str">
-        <v>KONICA MINOLTA TONER 2300 BLACK ΣΥΜΒΑΤΟ 4000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
+        <v>EPSON INK No 26XL - T2634XL YELLOW ΣΥΜΒΑΤΟ 10ml</v>
+      </c>
+      <c r="K4" t="str">
+        <v>20</v>
       </c>
       <c r="L4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v>GPT-0142</v>
+      </c>
+      <c r="J5" t="str">
+        <v>HP TONER CF383A MAGENTA ΣΥΜΒΑΤΟ 2700 ΣΕΛΙΔΕΣ</v>
+      </c>
+      <c r="K5" t="str">
+        <v>78</v>
+      </c>
+      <c r="L5" t="str">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Product List, Cost Decoration and Basic Login Form
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -442,16 +442,16 @@
         <v>ΦΛΕΜΙΝΓΚ ΚΑΙ ΠΕΡΙΦ ΟΔΟΣ 0</v>
       </c>
       <c r="I2" t="str">
-        <v>GPT-0532</v>
+        <v>GPI-0224</v>
       </c>
       <c r="J2" t="str">
-        <v>OKI TONER M C3100/3000/3200/5100/5150/5200/5300/5400/5510 MAGENTA ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
+        <v>CANON INK CLI-551XL GRAY ΣΥΜΒΑΤΟ 13ml</v>
       </c>
       <c r="K2" t="str">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="L2" t="str">
-        <v>1023.78€</v>
+        <v>780€</v>
       </c>
     </row>
     <row r="3">
@@ -480,13 +480,13 @@
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>GPI-0134</v>
+        <v>GPI-0023</v>
       </c>
       <c r="J3" t="str">
-        <v>HP INK No 88XL -  C9392A MAGENTA ΣΥΜΒΑΤΟ 28ml</v>
+        <v>EPSON INK No 26XL - T2634XL YELLOW ΣΥΜΒΑΤΟ 10ml</v>
       </c>
       <c r="K3" t="str">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="L3" t="str">
         <v/>
@@ -518,53 +518,15 @@
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>GPI-0023</v>
+        <v>GPT-0070</v>
       </c>
       <c r="J4" t="str">
-        <v>EPSON INK No 26XL - T2634XL YELLOW ΣΥΜΒΑΤΟ 10ml</v>
+        <v>EPSON TONER EPL6200L BLACK ΣΥΜΒΑΤΟ 6000 ΣΕΛΙΔΕΣ</v>
       </c>
       <c r="K4" t="str">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="L4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-      <c r="B5" t="str">
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v>GPT-0142</v>
-      </c>
-      <c r="J5" t="str">
-        <v>HP TONER CF383A MAGENTA ΣΥΜΒΑΤΟ 2700 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="K5" t="str">
-        <v>78</v>
-      </c>
-      <c r="L5" t="str">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Login Form and Field Validation
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,13 +410,13 @@
         <v>Διεύθυνση</v>
       </c>
       <c r="J1" t="str">
-        <v>Product ID</v>
+        <v>ΚΩΔΙΚΟΣ ΠΡΟΙΟΝΤΟΣ</v>
       </c>
       <c r="K1" t="str">
-        <v>Product Name</v>
+        <v>ΟΝΟΜΑ ΠΡΟΙΟΝΤΟΣ</v>
       </c>
       <c r="L1" t="str">
-        <v>Product Amount</v>
+        <v>ΠΟΣΟΤΗΤΑ ΠΡΟΙΟΝΤΟΣ</v>
       </c>
       <c r="M1" t="str">
         <v>Total Cost</v>
@@ -424,34 +424,37 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>SPOT4TONER Ι Κ Ε</v>
+        <v>ΜΩΡΑΙΤΗ  ΜΑΡΙΑ ΑΘΑΝΑΣΙΟΣ</v>
       </c>
       <c r="B2" t="str">
         <v>ΕΛΤΑ COURIER</v>
       </c>
       <c r="C2" t="str">
-        <v>800839540</v>
+        <v>055472412</v>
+      </c>
+      <c r="E2" t="str">
+        <v>2610433413</v>
       </c>
       <c r="G2" t="str">
-        <v>54621</v>
+        <v>26441</v>
       </c>
       <c r="H2" t="str">
-        <v>ΘΕΣΣΑΛΟΝΙΚΗ</v>
+        <v>ΠΑΤΡΑ</v>
       </c>
       <c r="I2" t="str">
-        <v>ΑΓΓΕΛΑΚΗ 3</v>
+        <v>ΑΓΙΑΣ ΣΟΦΙΑΣ 15</v>
       </c>
       <c r="J2" t="str">
-        <v>GPT-0533</v>
+        <v>GPT-0033</v>
       </c>
       <c r="K2" t="str">
-        <v>OKI TONER Y C3100/3000/3200/5100/5150/5200/5300/5400/5510 YELLOW ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
-      </c>
-      <c r="L2">
-        <v>3</v>
+        <v>SAMSUNG TONER CLP325/CLP320/4072 MAGENTA ΣΥΜΒΑΤΟ 1000 ΣΕΛΙΔΕΣ</v>
+      </c>
+      <c r="L2" t="str">
+        <v>15</v>
       </c>
       <c r="M2" t="str">
-        <v>10€</v>
+        <v>1055€</v>
       </c>
     </row>
     <row r="3">
@@ -483,15 +486,56 @@
         <v/>
       </c>
       <c r="J3" t="str">
-        <v>GPI-0076</v>
+        <v>GPI-0222</v>
       </c>
       <c r="K3" t="str">
-        <v>CANON INK CLI-526 MAGENTA ΣΥΜΒΑΤΟ 11ml</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
+        <v>HP INK No 971XL MAGENTA ΣΥΜΒΑΤΟ 120ml</v>
+      </c>
+      <c r="L3" t="str">
+        <v>98</v>
       </c>
       <c r="M3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v>GPI-0252</v>
+      </c>
+      <c r="K4" t="str">
+        <v>CANON INK CLI-571XL BLACK ΣΥΜΒΑΤΟ 13ml</v>
+      </c>
+      <c r="L4" t="str">
+        <v>163</v>
+      </c>
+      <c r="M4" t="str">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Heroku Password and Office email, Excel Exporting fix
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,22 +430,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>ΤΑΤΣΗΣ  ΓΕΩΡΓΙΟΣ</v>
+        <v>SPOT4TONER Ι Κ Ε</v>
       </c>
       <c r="B2" t="str">
-        <v>134312928</v>
-      </c>
-      <c r="D2" t="str">
-        <v>2681071591</v>
+        <v>800839540</v>
       </c>
       <c r="F2" t="str">
-        <v>47100</v>
+        <v>54621</v>
       </c>
       <c r="G2" t="str">
-        <v>ΑΡΤΑ</v>
+        <v>ΘΕΣΣΑΛΟΝΙΚΗ</v>
       </c>
       <c r="H2" t="str">
-        <v>ΦΛΕΜΙΝΓΚ ΚΑΙ ΠΕΡΙΦ ΟΔΟΣ 0</v>
+        <v>ΑΓΓΕΛΑΚΗ 3</v>
       </c>
       <c r="I2" t="str">
         <v>ΕΛΤΑ COURIER</v>
@@ -457,10 +454,57 @@
         <v>OKI TONER M C3100/3000/3200/5100/5150/5200/5300/5400/5510 MAGENTA ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O2" t="str">
-        <v>3€</v>
+        <v>45€</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v>GPT-0535</v>
+      </c>
+      <c r="M3" t="str">
+        <v>OKI TONER B432 BLACK ΣΥΜΒΑΤΟ 12000  ΣΕΛΙΔΕΣ</v>
+      </c>
+      <c r="N3" t="str">
+        <v>15</v>
+      </c>
+      <c r="O3" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polishing, Solving some Perfomance issues  and ... other stuff
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,28 +430,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>APOSTOLIS ANASTASIOU</v>
+        <v>ΑΠΟΣΤΟΛΟΣ ΑΝΑΣΤΑΣΙΟΥ</v>
       </c>
       <c r="B2" t="str">
-        <v>121212</v>
+        <v>6362</v>
       </c>
       <c r="C2" t="str">
-        <v>123123123123</v>
+        <v>6363</v>
       </c>
       <c r="D2" t="str">
         <v>6975362321</v>
       </c>
       <c r="E2" t="str">
-        <v>6975362321</v>
+        <v/>
       </c>
       <c r="F2" t="str">
-        <v>49100</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>lokation</v>
+        <v/>
       </c>
       <c r="H2" t="str">
-        <v>Kaiser Bridge</v>
+        <v/>
       </c>
       <c r="I2" t="str">
         <v>ΕΛΤΑ</v>
@@ -463,16 +463,16 @@
         <v>test</v>
       </c>
       <c r="L2" t="str">
-        <v>GPI-0138</v>
+        <v>DTS-0019</v>
       </c>
       <c r="M2" t="str">
-        <v>BROTHER INK LC1240 MAGENTA ΣΥΜΒΑΤΟ 10ml</v>
-      </c>
-      <c r="N2" t="str">
-        <v>12</v>
+        <v>ΣΥΜΒΑΤΗ ΜΕΛΑΝΟΤΑΙΝΙΑ EPSON ERC-32B BLACK</v>
+      </c>
+      <c r="N2">
+        <v>15</v>
       </c>
       <c r="O2" t="str">
-        <v>150€</v>
+        <v>20€</v>
       </c>
     </row>
     <row r="3">
@@ -510,156 +510,15 @@
         <v/>
       </c>
       <c r="L3" t="str">
-        <v>GPI-0136</v>
+        <v>GPI-0137</v>
       </c>
       <c r="M3" t="str">
-        <v>BROTHER INK LC1240 BLACK ΣΥΜΒΑΤΟ 20ml</v>
-      </c>
-      <c r="N3" t="str">
-        <v>72</v>
+        <v>BROTHER INK LC1240 CYAN ΣΥΜΒΑΤΟ 10ml</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
       </c>
       <c r="O3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v/>
-      </c>
-      <c r="B4" t="str">
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v>GPI-0194</v>
-      </c>
-      <c r="M4" t="str">
-        <v>EPSON INK T0613 MAGENTA ΣΥΜΒΑΤΟ 13.5ml</v>
-      </c>
-      <c r="N4" t="str">
-        <v>88</v>
-      </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-      <c r="B5" t="str">
-        <v/>
-      </c>
-      <c r="C5" t="str">
-        <v/>
-      </c>
-      <c r="D5" t="str">
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v>GPI-0112</v>
-      </c>
-      <c r="M5" t="str">
-        <v>CANON INK PG-512 BLACK ΣΥΜΒΑΤΟ 14ml</v>
-      </c>
-      <c r="N5" t="str">
-        <v>1</v>
-      </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v/>
-      </c>
-      <c r="B6" t="str">
-        <v/>
-      </c>
-      <c r="C6" t="str">
-        <v/>
-      </c>
-      <c r="D6" t="str">
-        <v/>
-      </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v/>
-      </c>
-      <c r="H6" t="str">
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <v>GPI-0116</v>
-      </c>
-      <c r="M6" t="str">
-        <v>HP INK No 336XL - C9362E BLACK ΣΥΜΒΑΤΟ 20ml</v>
-      </c>
-      <c r="N6" t="str">
-        <v>3</v>
-      </c>
-      <c r="O6" t="str">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Sending to Multiple Emails
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Data"/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,63 +463,16 @@
         <v>test</v>
       </c>
       <c r="L2" t="str">
-        <v>DTS-0019</v>
+        <v>GPT-0532</v>
       </c>
       <c r="M2" t="str">
-        <v>ΣΥΜΒΑΤΗ ΜΕΛΑΝΟΤΑΙΝΙΑ EPSON ERC-32B BLACK</v>
+        <v>OKI TONER M C3100/3000/3200/5100/5150/5200/5300/5400/5510 MAGENTA ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
       </c>
       <c r="N2">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="O2" t="str">
-        <v>20€</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v/>
-      </c>
-      <c r="B3" t="str">
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
-      <c r="E3" t="str">
-        <v/>
-      </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="str">
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v/>
-      </c>
-      <c r="L3" t="str">
-        <v>GPI-0137</v>
-      </c>
-      <c r="M3" t="str">
-        <v>BROTHER INK LC1240 CYAN ΣΥΜΒΑΤΟ 10ml</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
-      <c r="O3" t="str">
-        <v/>
+        <v>4€</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Polish, I guess ...
</commit_message>
<xml_diff>
--- a/server/files/formData.xlsx
+++ b/server/files/formData.xlsx
@@ -469,10 +469,10 @@
         <v>OKI TONER M C3100/3000/3200/5100/5150/5200/5300/5400/5510 MAGENTA ΣΥΜΒΑΤΟ 3000 ΣΕΛΙΔΕΣ</v>
       </c>
       <c r="N2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O2" t="str">
-        <v>4€</v>
+        <v>3€</v>
       </c>
     </row>
   </sheetData>

</xml_diff>